<commit_message>
Working, finally, on my machine
Need to comment DfReadDataFile.R and ReadJAFROCNewFormat.R and add more checks in the code for illegal values; the sorting introduced all sorts of problems; sorted caseID column is used now in only 3 places;
k <- which(unique(truthTableSort$CaseID) == truthTable$CaseID[l])
k <- which(unique(truthTableSort$CaseID) == NLCaseIDCol[l])
k <- which(unique(truthTableSort$CaseID) == LLCaseIDCol[l]) - K1
Also need to update NEWS.md;
</commit_message>
<xml_diff>
--- a/inst/extdata/toyFiles/FROC/frocSpA.xlsx
+++ b/inst/extdata/toyFiles/FROC/frocSpA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dev/GitHub/RJafroc/inst/extdata/toyFiles/ROC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dev/GitHub/RJafroc/inst/extdata/toyFiles/FROC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3F725BC-25BC-1E45-9672-CB65BCB84AD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B79460-3BCA-1E4B-ABD1-F3FA4D2DEB3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13060" yWindow="740" windowWidth="10580" windowHeight="12600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38660" yWindow="13540" windowWidth="10580" windowHeight="12600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TP" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="20">
   <si>
     <t>CaseID</t>
   </si>
@@ -1039,8 +1039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1686,8 +1686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1950,8 +1950,8 @@
       <c r="A15" s="2">
         <v>19</v>
       </c>
-      <c r="B15" s="2">
-        <v>1</v>
+      <c r="B15" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="C15" s="2">
         <v>0</v>
@@ -2239,8 +2239,8 @@
       <c r="A32" s="2">
         <v>19</v>
       </c>
-      <c r="B32" s="2">
-        <v>1</v>
+      <c r="B32" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="C32" s="2">
         <v>0</v>
@@ -2307,7 +2307,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <ignoredErrors>
-    <ignoredError sqref="E18:E22 E2:E7 B8:B18 E15 E12:E13 E8:E11 E14 E16:E17 E23:E35 B25:B35" numberStoredAsText="1"/>
+    <ignoredError sqref="E18:E22 E2:E7 B8:B15 E15 E12:E13 E8:E11 E14 E16:E17 E23:E35 B25:B32 B16:B18 B33:B35" numberStoredAsText="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
Read actual SPLIT-PLOT-A dataset
* Did not find any data entry errors in `/toyFiles/FROC/1T3Rvs4R.xlsx`
* Simplified `rdrArr` handling: this is done in `checkTruthTable`, where SPLIT-PLOT-A is handled separately;
* Passes all tests
* Next: implement the formulae, i.e. Cov2; found out how to estimate Cov2 by averaging multiple sample estimates
</commit_message>
<xml_diff>
--- a/inst/extdata/toyFiles/FROC/frocSpA.xlsx
+++ b/inst/extdata/toyFiles/FROC/frocSpA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dev/GitHub/RJafroc/inst/extdata/toyFiles/FROC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B79460-3BCA-1E4B-ABD1-F3FA4D2DEB3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4C79174-FE63-7F4D-87E8-5223597828BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38660" yWindow="13540" windowWidth="10580" windowHeight="12600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39140" yWindow="15260" windowWidth="10580" windowHeight="12600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TP" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="21">
   <si>
     <t>CaseID</t>
   </si>
@@ -71,9 +71,6 @@
     <t>1,  2</t>
   </si>
   <si>
-    <t>3,  4</t>
-  </si>
-  <si>
     <t>FROC</t>
   </si>
   <si>
@@ -93,6 +90,12 @@
   </si>
   <si>
     <t>1.9</t>
+  </si>
+  <si>
+    <t>3,  4, 5</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
 </sst>
 </file>
@@ -124,12 +127,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -244,7 +253,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -259,6 +268,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="101">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -655,10 +668,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD21"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1024,9 +1037,97 @@
         <v>5.3</v>
       </c>
     </row>
+    <row r="22" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="6">
+        <v>16</v>
+      </c>
+      <c r="D22" s="6">
+        <v>1</v>
+      </c>
+      <c r="E22" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="3">
+        <v>17</v>
+      </c>
+      <c r="D23" s="3">
+        <v>1</v>
+      </c>
+      <c r="E23" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="3">
+        <v>18</v>
+      </c>
+      <c r="D24" s="3">
+        <v>1</v>
+      </c>
+      <c r="E24" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="3">
+        <v>19</v>
+      </c>
+      <c r="D25" s="3">
+        <v>1</v>
+      </c>
+      <c r="E25" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="3">
+        <v>20</v>
+      </c>
+      <c r="D26" s="3">
+        <v>1</v>
+      </c>
+      <c r="E26" s="3">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <ignoredErrors>
+    <ignoredError sqref="A22:A27 B22:B26" numberStoredAsText="1"/>
+  </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1037,10 +1138,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44:A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1444,7 +1545,7 @@
         <v>16</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -1458,7 +1559,7 @@
         <v>16</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -1472,7 +1573,7 @@
         <v>16</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -1517,7 +1618,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>2</v>
       </c>
@@ -1531,7 +1632,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>3</v>
       </c>
@@ -1545,7 +1646,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>3</v>
       </c>
@@ -1559,7 +1660,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>3</v>
       </c>
@@ -1573,7 +1674,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>3</v>
       </c>
@@ -1587,7 +1688,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>3</v>
       </c>
@@ -1601,7 +1702,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>4</v>
       </c>
@@ -1615,7 +1716,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>4</v>
       </c>
@@ -1629,7 +1730,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>4</v>
       </c>
@@ -1643,7 +1744,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>4</v>
       </c>
@@ -1657,7 +1758,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>4</v>
       </c>
@@ -1669,11 +1770,159 @@
       </c>
       <c r="D43" s="3">
         <v>5.3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B44" s="3">
+        <v>2</v>
+      </c>
+      <c r="C44" s="3">
+        <v>6</v>
+      </c>
+      <c r="D44" s="3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E44" s="3"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B45" s="3">
+        <v>2</v>
+      </c>
+      <c r="C45" s="3">
+        <v>7</v>
+      </c>
+      <c r="D45" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="E45" s="3"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B46" s="3">
+        <v>2</v>
+      </c>
+      <c r="C46" s="3">
+        <v>8</v>
+      </c>
+      <c r="D46" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="E46" s="3"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B47" s="3">
+        <v>2</v>
+      </c>
+      <c r="C47" s="3">
+        <v>9</v>
+      </c>
+      <c r="D47" s="3">
+        <v>5.6</v>
+      </c>
+      <c r="E47" s="3"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B48" s="3">
+        <v>2</v>
+      </c>
+      <c r="C48" s="3">
+        <v>10</v>
+      </c>
+      <c r="D48" s="3">
+        <v>3.4</v>
+      </c>
+      <c r="E48" s="3"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B49" s="3">
+        <v>2</v>
+      </c>
+      <c r="C49" s="3">
+        <v>16</v>
+      </c>
+      <c r="D49" s="3">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B50" s="3">
+        <v>2</v>
+      </c>
+      <c r="C50" s="3">
+        <v>17</v>
+      </c>
+      <c r="D50" s="3">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B51" s="3">
+        <v>2</v>
+      </c>
+      <c r="C51" s="3">
+        <v>18</v>
+      </c>
+      <c r="D51" s="3">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B52" s="3">
+        <v>2</v>
+      </c>
+      <c r="C52" s="3">
+        <v>19</v>
+      </c>
+      <c r="D52" s="3">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B53" s="3">
+        <v>2</v>
+      </c>
+      <c r="C53" s="3">
+        <v>20</v>
+      </c>
+      <c r="D53" s="3">
+        <v>4.7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <ignoredErrors>
+    <ignoredError sqref="A44:A53" numberStoredAsText="1"/>
+  </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1686,8 +1935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1736,7 +1985,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1832,7 +2081,7 @@
         <v>16</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" s="2">
         <v>0</v>
@@ -1866,7 +2115,7 @@
         <v>17</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="2">
         <v>0</v>
@@ -1883,7 +2132,7 @@
         <v>17</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="2">
         <v>0</v>
@@ -1900,7 +2149,7 @@
         <v>17</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="2">
         <v>0</v>
@@ -1951,7 +2200,7 @@
         <v>19</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" s="2">
         <v>0</v>
@@ -1985,7 +2234,7 @@
         <v>20</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17" s="2">
         <v>0</v>
@@ -2002,7 +2251,7 @@
         <v>20</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18" s="2">
         <v>0</v>
@@ -2025,7 +2274,7 @@
         <v>0</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>9</v>
@@ -2042,7 +2291,7 @@
         <v>0</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>9</v>
@@ -2059,7 +2308,7 @@
         <v>0</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>9</v>
@@ -2076,7 +2325,7 @@
         <v>0</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>9</v>
@@ -2093,7 +2342,7 @@
         <v>0</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>9</v>
@@ -2110,7 +2359,7 @@
         <v>0</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>9</v>
@@ -2121,13 +2370,13 @@
         <v>16</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C25" s="2">
         <v>0</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>9</v>
@@ -2144,7 +2393,7 @@
         <v>0</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>9</v>
@@ -2155,13 +2404,13 @@
         <v>17</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C27" s="2">
         <v>0</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>9</v>
@@ -2172,13 +2421,13 @@
         <v>17</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C28" s="2">
         <v>0</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>9</v>
@@ -2189,13 +2438,13 @@
         <v>17</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C29" s="2">
         <v>0</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>9</v>
@@ -2212,7 +2461,7 @@
         <v>0</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>9</v>
@@ -2229,7 +2478,7 @@
         <v>0</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>9</v>
@@ -2240,13 +2489,13 @@
         <v>19</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C32" s="2">
         <v>0</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>9</v>
@@ -2263,7 +2512,7 @@
         <v>0</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>9</v>
@@ -2274,13 +2523,13 @@
         <v>20</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C34" s="2">
         <v>0</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>9</v>
@@ -2291,13 +2540,13 @@
         <v>20</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C35" s="2">
         <v>0</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
While it is working, I need to document changes in NEWS.md
Chk MaxNLF vs. JAFROC
Chk indexing with SpA dataset
Chk indexing with SpC dataset
Chk indexing with Factorial dataset
Modify SpA dataset to have unequal numbers of cases
</commit_message>
<xml_diff>
--- a/inst/extdata/toyFiles/FROC/frocSpA.xlsx
+++ b/inst/extdata/toyFiles/FROC/frocSpA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dev/GitHub/RJafroc/inst/extdata/toyFiles/FROC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B70C5B-E6F2-134D-B30D-3386F2A5A8AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4563E115-BCA2-C148-B7E4-F07BDFAC488B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="1640" windowWidth="10580" windowHeight="19440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8640" yWindow="2960" windowWidth="10580" windowHeight="19440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TP" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="39">
   <si>
     <t>CaseID</t>
   </si>
@@ -137,6 +137,21 @@
   </si>
   <si>
     <t>2.1</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>3.2</t>
+  </si>
+  <si>
+    <t>4.1</t>
+  </si>
+  <si>
+    <t>2.9</t>
+  </si>
+  <si>
+    <t>16</t>
   </si>
 </sst>
 </file>
@@ -457,8 +472,8 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>80220</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:aink="http://schemas.microsoft.com/office/drawing/2016/ink" Requires="xdr14 aink">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:aink="http://schemas.microsoft.com/office/drawing/2016/ink">
+      <mc:Choice Requires="xdr14 aink">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="2" name="Ink 1">
@@ -477,7 +492,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="2" name="Ink 1">
@@ -522,8 +537,8 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>100740</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:aink="http://schemas.microsoft.com/office/drawing/2016/ink" Requires="xdr14 aink">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:aink="http://schemas.microsoft.com/office/drawing/2016/ink">
+      <mc:Choice Requires="xdr14 aink">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="3" name="Ink 2">
@@ -542,7 +557,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="3" name="Ink 2">
@@ -578,17 +593,17 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>331840</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>45780</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>332200</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>46140</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:aink="http://schemas.microsoft.com/office/drawing/2016/ink" Requires="xdr14 aink">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:aink="http://schemas.microsoft.com/office/drawing/2016/ink">
+      <mc:Choice Requires="xdr14 aink">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="4" name="Ink 3">
@@ -607,7 +622,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="4" name="Ink 3">
@@ -643,17 +658,17 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>282180</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>115620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>322860</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>129660</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:aink="http://schemas.microsoft.com/office/drawing/2016/ink" Requires="xdr14 aink">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:aink="http://schemas.microsoft.com/office/drawing/2016/ink">
+      <mc:Choice Requires="xdr14 aink">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="7" name="Ink 6">
@@ -672,7 +687,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="7" name="Ink 6">
@@ -1099,10 +1114,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1393,28 +1408,28 @@
       <c r="C17" s="3">
         <v>16</v>
       </c>
-      <c r="D17" s="3">
-        <v>1</v>
+      <c r="D17" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="E17" s="3">
         <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="3">
-        <v>4</v>
-      </c>
-      <c r="B18" s="3">
-        <v>2</v>
-      </c>
-      <c r="C18" s="3">
-        <v>17</v>
-      </c>
-      <c r="D18" s="3">
-        <v>1</v>
-      </c>
-      <c r="E18" s="3">
-        <v>5.3</v>
+      <c r="A18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1425,13 +1440,13 @@
         <v>2</v>
       </c>
       <c r="C19" s="3">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D19" s="3">
         <v>1</v>
       </c>
       <c r="E19" s="3">
-        <v>5.2</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -1442,13 +1457,13 @@
         <v>2</v>
       </c>
       <c r="C20" s="3">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D20" s="3">
         <v>1</v>
       </c>
       <c r="E20" s="3">
-        <v>3.1</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -1459,33 +1474,33 @@
         <v>2</v>
       </c>
       <c r="C21" s="3">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D21" s="3">
         <v>1</v>
       </c>
       <c r="E21" s="3">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
+        <v>4</v>
+      </c>
+      <c r="B22" s="3">
+        <v>2</v>
+      </c>
+      <c r="C22" s="3">
+        <v>20</v>
+      </c>
+      <c r="D22" s="3">
+        <v>1</v>
+      </c>
+      <c r="E22" s="3">
         <v>5.3</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="3">
-        <v>16</v>
-      </c>
-      <c r="D22" s="3">
-        <v>1</v>
-      </c>
-      <c r="E22" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
@@ -1493,13 +1508,13 @@
         <v>13</v>
       </c>
       <c r="C23" s="3">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D23" s="3">
         <v>1</v>
       </c>
       <c r="E23" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -1510,13 +1525,13 @@
         <v>13</v>
       </c>
       <c r="C24" s="3">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D24" s="3">
         <v>1</v>
       </c>
       <c r="E24" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -1527,13 +1542,13 @@
         <v>13</v>
       </c>
       <c r="C25" s="3">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D25" s="3">
         <v>1</v>
       </c>
       <c r="E25" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -1544,29 +1559,46 @@
         <v>13</v>
       </c>
       <c r="C26" s="3">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D26" s="3">
         <v>1</v>
       </c>
       <c r="E26" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="3">
+        <v>20</v>
+      </c>
+      <c r="D27" s="3">
+        <v>1</v>
+      </c>
+      <c r="E27" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B27" s="1" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1574,7 +1606,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <ignoredErrors>
-    <ignoredError sqref="A22:A26 B22:B26 A4:E4 A27:E27" numberStoredAsText="1"/>
+    <ignoredError sqref="A23:A27 B23:B27 A4:E4 A28:E28 D17:D18 A18:C18" numberStoredAsText="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -1586,10 +1618,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25:D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1688,47 +1720,47 @@
       <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="7">
-        <v>1</v>
-      </c>
-      <c r="B7" s="7">
-        <v>4</v>
-      </c>
-      <c r="C7" s="7">
+      <c r="A7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="7">
+        <v>1</v>
+      </c>
+      <c r="B9" s="7">
+        <v>4</v>
+      </c>
+      <c r="C9" s="7">
         <v>10</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D9" s="7" t="s">
         <v>16</v>
-      </c>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
-        <v>2</v>
-      </c>
-      <c r="B8" s="3">
-        <v>4</v>
-      </c>
-      <c r="C8" s="3">
-        <v>6</v>
-      </c>
-      <c r="D8" s="3">
-        <v>0.9</v>
-      </c>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
-        <v>2</v>
-      </c>
-      <c r="B9" s="3">
-        <v>4</v>
-      </c>
-      <c r="C9" s="3">
-        <v>7</v>
-      </c>
-      <c r="D9" s="3">
-        <v>1.3</v>
       </c>
       <c r="E9" s="3"/>
     </row>
@@ -1740,10 +1772,10 @@
         <v>4</v>
       </c>
       <c r="C10" s="3">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D10" s="3">
-        <v>1.5</v>
+        <v>0.9</v>
       </c>
       <c r="E10" s="3"/>
     </row>
@@ -1755,10 +1787,10 @@
         <v>4</v>
       </c>
       <c r="C11" s="3">
-        <v>9</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>18</v>
+        <v>7</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1.3</v>
       </c>
       <c r="E11" s="3"/>
     </row>
@@ -1770,40 +1802,40 @@
         <v>4</v>
       </c>
       <c r="C12" s="3">
+        <v>8</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <v>2</v>
+      </c>
+      <c r="B13" s="3">
+        <v>4</v>
+      </c>
+      <c r="C13" s="3">
+        <v>9</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <v>2</v>
+      </c>
+      <c r="B14" s="3">
+        <v>4</v>
+      </c>
+      <c r="C14" s="3">
         <v>10</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D14" s="3">
         <v>5.5</v>
-      </c>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="8">
-        <v>3</v>
-      </c>
-      <c r="B13" s="8">
-        <v>2</v>
-      </c>
-      <c r="C13" s="8">
-        <v>6</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="8">
-        <v>3</v>
-      </c>
-      <c r="B14" s="8">
-        <v>2</v>
-      </c>
-      <c r="C14" s="8">
-        <v>7</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="E14" s="3"/>
     </row>
@@ -1815,10 +1847,10 @@
         <v>2</v>
       </c>
       <c r="C15" s="8">
-        <v>8</v>
-      </c>
-      <c r="D15" s="8">
-        <v>1.3</v>
+        <v>6</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="E15" s="3"/>
     </row>
@@ -1830,10 +1862,10 @@
         <v>2</v>
       </c>
       <c r="C16" s="8">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E16" s="3"/>
     </row>
@@ -1845,39 +1877,39 @@
         <v>2</v>
       </c>
       <c r="C17" s="8">
+        <v>8</v>
+      </c>
+      <c r="D17" s="8">
+        <v>1.3</v>
+      </c>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="8">
+        <v>3</v>
+      </c>
+      <c r="B18" s="8">
+        <v>2</v>
+      </c>
+      <c r="C18" s="8">
+        <v>9</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="8">
+        <v>3</v>
+      </c>
+      <c r="B19" s="8">
+        <v>2</v>
+      </c>
+      <c r="C19" s="8">
         <v>10</v>
       </c>
-      <c r="D17" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="3">
-        <v>4</v>
-      </c>
-      <c r="B18" s="3">
-        <v>2</v>
-      </c>
-      <c r="C18" s="3">
-        <v>6</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E18" s="3"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="3">
-        <v>4</v>
-      </c>
-      <c r="B19" s="3">
-        <v>2</v>
-      </c>
-      <c r="C19" s="3">
-        <v>7</v>
-      </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="8" t="s">
         <v>29</v>
       </c>
       <c r="E19" s="3"/>
@@ -1890,10 +1922,10 @@
         <v>2</v>
       </c>
       <c r="C20" s="3">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E20" s="3"/>
     </row>
@@ -1905,10 +1937,10 @@
         <v>2</v>
       </c>
       <c r="C21" s="3">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E21" s="3"/>
     </row>
@@ -1920,67 +1952,69 @@
         <v>2</v>
       </c>
       <c r="C22" s="3">
+        <v>8</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
+        <v>4</v>
+      </c>
+      <c r="B23" s="3">
+        <v>2</v>
+      </c>
+      <c r="C23" s="3">
+        <v>9</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
+        <v>4</v>
+      </c>
+      <c r="B24" s="3">
+        <v>2</v>
+      </c>
+      <c r="C24" s="3">
         <v>10</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D24" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E22" s="3"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="7">
-        <v>1</v>
-      </c>
-      <c r="B23" s="7">
-        <v>4</v>
-      </c>
-      <c r="C23" s="7">
-        <v>16</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="7">
-        <v>1</v>
-      </c>
-      <c r="B24" s="7">
-        <v>4</v>
-      </c>
-      <c r="C24" s="7">
-        <v>17</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>30</v>
-      </c>
+      <c r="E24" s="3"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="7">
-        <v>1</v>
-      </c>
-      <c r="B25" s="7">
-        <v>4</v>
-      </c>
-      <c r="C25" s="7">
-        <v>18</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>16</v>
+      <c r="A25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="3">
+        <v>2</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="7">
-        <v>1</v>
-      </c>
-      <c r="B26" s="7">
-        <v>4</v>
-      </c>
-      <c r="C26" s="7">
-        <v>19</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>21</v>
+      <c r="A26" s="3">
+        <v>4</v>
+      </c>
+      <c r="B26" s="3">
+        <v>2</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -1991,66 +2025,66 @@
         <v>4</v>
       </c>
       <c r="C27" s="7">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D27" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="7">
+        <v>1</v>
+      </c>
+      <c r="B28" s="7">
+        <v>4</v>
+      </c>
+      <c r="C28" s="7">
+        <v>17</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="7">
+        <v>1</v>
+      </c>
+      <c r="B29" s="7">
+        <v>4</v>
+      </c>
+      <c r="C29" s="7">
+        <v>18</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="7">
+        <v>1</v>
+      </c>
+      <c r="B30" s="7">
+        <v>4</v>
+      </c>
+      <c r="C30" s="7">
+        <v>19</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="7">
+        <v>1</v>
+      </c>
+      <c r="B31" s="7">
+        <v>4</v>
+      </c>
+      <c r="C31" s="7">
+        <v>20</v>
+      </c>
+      <c r="D31" s="7" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="3">
-        <v>2</v>
-      </c>
-      <c r="B28" s="3">
-        <v>4</v>
-      </c>
-      <c r="C28" s="3">
-        <v>16</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="3">
-        <v>2</v>
-      </c>
-      <c r="B29" s="3">
-        <v>4</v>
-      </c>
-      <c r="C29" s="3">
-        <v>16</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="3">
-        <v>2</v>
-      </c>
-      <c r="B30" s="3">
-        <v>4</v>
-      </c>
-      <c r="C30" s="3">
-        <v>16</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="3">
-        <v>2</v>
-      </c>
-      <c r="B31" s="3">
-        <v>4</v>
-      </c>
-      <c r="C31" s="3">
-        <v>17</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -2061,10 +2095,10 @@
         <v>4</v>
       </c>
       <c r="C32" s="3">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -2075,10 +2109,10 @@
         <v>4</v>
       </c>
       <c r="C33" s="3">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -2089,66 +2123,66 @@
         <v>4</v>
       </c>
       <c r="C34" s="3">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D34" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="3">
+        <v>2</v>
+      </c>
+      <c r="B35" s="3">
+        <v>4</v>
+      </c>
+      <c r="C35" s="3">
+        <v>17</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="8">
-        <v>3</v>
-      </c>
-      <c r="B35" s="8">
-        <v>2</v>
-      </c>
-      <c r="C35" s="8">
-        <v>16</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="8">
-        <v>3</v>
-      </c>
-      <c r="B36" s="8">
-        <v>2</v>
-      </c>
-      <c r="C36" s="8">
-        <v>17</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>16</v>
+      <c r="A36" s="3">
+        <v>2</v>
+      </c>
+      <c r="B36" s="3">
+        <v>4</v>
+      </c>
+      <c r="C36" s="3">
+        <v>18</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>16</v>
+      <c r="A37" s="3">
+        <v>2</v>
+      </c>
+      <c r="B37" s="3">
+        <v>4</v>
+      </c>
+      <c r="C37" s="3">
+        <v>19</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="8">
-        <v>3</v>
-      </c>
-      <c r="B38" s="8">
-        <v>2</v>
-      </c>
-      <c r="C38" s="8">
-        <v>18</v>
-      </c>
-      <c r="D38" s="8">
-        <v>5.2</v>
+      <c r="A38" s="3">
+        <v>2</v>
+      </c>
+      <c r="B38" s="3">
+        <v>4</v>
+      </c>
+      <c r="C38" s="3">
+        <v>20</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -2159,10 +2193,10 @@
         <v>2</v>
       </c>
       <c r="C39" s="8">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -2173,66 +2207,66 @@
         <v>2</v>
       </c>
       <c r="C40" s="8">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D40" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="8">
+        <v>3</v>
+      </c>
+      <c r="B42" s="8">
+        <v>2</v>
+      </c>
+      <c r="C42" s="8">
+        <v>18</v>
+      </c>
+      <c r="D42" s="8">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="8">
+        <v>3</v>
+      </c>
+      <c r="B43" s="8">
+        <v>2</v>
+      </c>
+      <c r="C43" s="8">
+        <v>19</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="8">
+        <v>3</v>
+      </c>
+      <c r="B44" s="8">
+        <v>2</v>
+      </c>
+      <c r="C44" s="8">
+        <v>20</v>
+      </c>
+      <c r="D44" s="8" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="3">
-        <v>4</v>
-      </c>
-      <c r="B41" s="3">
-        <v>2</v>
-      </c>
-      <c r="C41" s="3">
-        <v>16</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="3">
-        <v>4</v>
-      </c>
-      <c r="B42" s="3">
-        <v>2</v>
-      </c>
-      <c r="C42" s="3">
-        <v>17</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="3">
-        <v>4</v>
-      </c>
-      <c r="B43" s="3">
-        <v>2</v>
-      </c>
-      <c r="C43" s="3">
-        <v>18</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="3">
-        <v>4</v>
-      </c>
-      <c r="B44" s="3">
-        <v>2</v>
-      </c>
-      <c r="C44" s="3">
-        <v>19</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -2243,69 +2277,67 @@
         <v>2</v>
       </c>
       <c r="C45" s="3">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D45" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="3">
+        <v>4</v>
+      </c>
+      <c r="B46" s="3">
+        <v>2</v>
+      </c>
+      <c r="C46" s="3">
         <v>17</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B46" s="3">
-        <v>2</v>
-      </c>
-      <c r="C46" s="3">
-        <v>6</v>
-      </c>
-      <c r="D46" s="3">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="E46" s="3"/>
+      <c r="D46" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
-        <v>20</v>
+      <c r="A47" s="3">
+        <v>4</v>
       </c>
       <c r="B47" s="3">
         <v>2</v>
       </c>
       <c r="C47" s="3">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E47" s="3"/>
+        <v>27</v>
+      </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="3" t="s">
-        <v>20</v>
+      <c r="A48" s="3">
+        <v>4</v>
       </c>
       <c r="B48" s="3">
         <v>2</v>
       </c>
       <c r="C48" s="3">
-        <v>8</v>
-      </c>
-      <c r="D48" s="3">
-        <v>1.3</v>
+        <v>19</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="E48" s="3"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" s="3" t="s">
-        <v>20</v>
+      <c r="A49" s="3">
+        <v>4</v>
       </c>
       <c r="B49" s="3">
         <v>2</v>
       </c>
       <c r="C49" s="3">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E49" s="3"/>
     </row>
@@ -2317,10 +2349,10 @@
         <v>2</v>
       </c>
       <c r="C50" s="3">
-        <v>10</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>29</v>
+        <v>6</v>
+      </c>
+      <c r="D50" s="3">
+        <v>2.2999999999999998</v>
       </c>
       <c r="E50" s="3"/>
     </row>
@@ -2332,11 +2364,12 @@
         <v>2</v>
       </c>
       <c r="C51" s="3">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>21</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="E51" s="3"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
@@ -2346,11 +2379,12 @@
         <v>2</v>
       </c>
       <c r="C52" s="3">
-        <v>17</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>16</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D52" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="E52" s="3"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
@@ -2360,10 +2394,10 @@
         <v>2</v>
       </c>
       <c r="C53" s="3">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -2374,10 +2408,10 @@
         <v>2</v>
       </c>
       <c r="C54" s="3">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -2388,9 +2422,65 @@
         <v>2</v>
       </c>
       <c r="C55" s="3">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D55" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B56" s="3">
+        <v>2</v>
+      </c>
+      <c r="C56" s="3">
+        <v>17</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B57" s="3">
+        <v>2</v>
+      </c>
+      <c r="C57" s="3">
+        <v>18</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B58" s="3">
+        <v>2</v>
+      </c>
+      <c r="C58" s="3">
+        <v>19</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B59" s="3">
+        <v>2</v>
+      </c>
+      <c r="C59" s="3">
+        <v>20</v>
+      </c>
+      <c r="D59" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2398,7 +2488,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <ignoredErrors>
-    <ignoredError sqref="A46:A55 D4:D55 D2 A3:D3" numberStoredAsText="1"/>
+    <ignoredError sqref="A50:A59 D27:D59 D2 A3:D3 D4:D6 A7:D8 D9:D24 C26 C25 D25:D26" numberStoredAsText="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -2410,10 +2500,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2537,11 +2627,11 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="6">
-        <v>16</v>
+      <c r="A7" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="B7" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="6">
         <v>0</v>
@@ -2557,8 +2647,8 @@
       <c r="A8" s="6">
         <v>16</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>13</v>
+      <c r="B8" s="6">
+        <v>1</v>
       </c>
       <c r="C8" s="6">
         <v>0</v>
@@ -2572,10 +2662,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
-        <v>17</v>
-      </c>
-      <c r="B9" s="6">
-        <v>1</v>
+        <v>16</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="C9" s="6">
         <v>0</v>
@@ -2591,8 +2681,8 @@
       <c r="A10" s="6">
         <v>17</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>13</v>
+      <c r="B10" s="6">
+        <v>1</v>
       </c>
       <c r="C10" s="6">
         <v>0</v>
@@ -2609,7 +2699,7 @@
         <v>17</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="6">
         <v>0</v>
@@ -2626,7 +2716,7 @@
         <v>17</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="6">
         <v>0</v>
@@ -2640,10 +2730,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
-        <v>18</v>
-      </c>
-      <c r="B13" s="6">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="C13" s="6">
         <v>0</v>
@@ -2657,7 +2747,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" s="6">
         <v>1</v>
@@ -2676,8 +2766,8 @@
       <c r="A15" s="6">
         <v>19</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>13</v>
+      <c r="B15" s="6">
+        <v>1</v>
       </c>
       <c r="C15" s="6">
         <v>0</v>
@@ -2691,10 +2781,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
-        <v>20</v>
-      </c>
-      <c r="B16" s="6">
-        <v>1</v>
+        <v>19</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="C16" s="6">
         <v>0</v>
@@ -2710,8 +2800,8 @@
       <c r="A17" s="6">
         <v>20</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>13</v>
+      <c r="B17" s="6">
+        <v>1</v>
       </c>
       <c r="C17" s="6">
         <v>0</v>
@@ -2728,7 +2818,7 @@
         <v>20</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18" s="6">
         <v>0</v>
@@ -2741,25 +2831,25 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
-        <v>6</v>
-      </c>
-      <c r="B19" s="2">
-        <v>0</v>
-      </c>
-      <c r="C19" s="2">
-        <v>0</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>19</v>
+      <c r="A19" s="6">
+        <v>20</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="6">
+        <v>0</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B20" s="2">
         <v>0</v>
@@ -2776,7 +2866,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B21" s="2">
         <v>0</v>
@@ -2793,7 +2883,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B22" s="2">
         <v>0</v>
@@ -2810,7 +2900,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B23" s="2">
         <v>0</v>
@@ -2827,10 +2917,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B24" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24" s="2">
         <v>0</v>
@@ -2843,13 +2933,13 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="2">
-        <v>16</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="2">
+      <c r="A25" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="6">
+        <v>0</v>
+      </c>
+      <c r="C25" s="6">
         <v>0</v>
       </c>
       <c r="D25" s="2" t="s">
@@ -2861,7 +2951,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B26" s="2">
         <v>1</v>
@@ -2878,7 +2968,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>13</v>
@@ -2897,8 +2987,8 @@
       <c r="A28" s="2">
         <v>17</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>14</v>
+      <c r="B28" s="2">
+        <v>1</v>
       </c>
       <c r="C28" s="2">
         <v>0</v>
@@ -2915,7 +3005,7 @@
         <v>17</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C29" s="2">
         <v>0</v>
@@ -2929,10 +3019,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
-        <v>18</v>
-      </c>
-      <c r="B30" s="2">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="C30" s="2">
         <v>0</v>
@@ -2946,10 +3036,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
-        <v>19</v>
-      </c>
-      <c r="B31" s="2">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C31" s="2">
         <v>0</v>
@@ -2963,10 +3053,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
-        <v>19</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>13</v>
+        <v>18</v>
+      </c>
+      <c r="B32" s="2">
+        <v>1</v>
       </c>
       <c r="C32" s="2">
         <v>0</v>
@@ -2980,7 +3070,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B33" s="2">
         <v>1</v>
@@ -2997,7 +3087,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>13</v>
@@ -3016,8 +3106,8 @@
       <c r="A35" s="2">
         <v>20</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>14</v>
+      <c r="B35" s="2">
+        <v>1</v>
       </c>
       <c r="C35" s="2">
         <v>0</v>
@@ -3026,6 +3116,40 @@
         <v>19</v>
       </c>
       <c r="E35" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="2">
+        <v>20</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="2">
+        <v>0</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="2">
+        <v>20</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E37" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -3033,7 +3157,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <ignoredErrors>
-    <ignoredError sqref="E18:E22 E2:E7 B8:B15 E15 E12:E13 E8:E11 E14 E16:E17 E23:E35 B25:B32 B16:B18 B33:B35" numberStoredAsText="1"/>
+    <ignoredError sqref="E26:E37 B9:B19 B27:B37 E2:E6 E7:E23 A7 E24:E25 A25" numberStoredAsText="1"/>
   </ignoredErrors>
   <drawing r:id="rId1"/>
   <extLst>

</xml_diff>